<commit_message>
find files by size linux
</commit_message>
<xml_diff>
--- a/DecisionTree/DecisionTreeBinary/BinaryCrossEntropy.xlsx
+++ b/DecisionTree/DecisionTreeBinary/BinaryCrossEntropy.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GD\DS\zOutros_Materiais\N\MateriaisParaEstudo\ArvoreDecisao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GD\DS\DS_Share\Github\DecisionTree\DecisionTreeBinary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288798D6-5C05-445F-91F0-2F78D987F051}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818897F7-C3A2-4F65-9561-DB2D202BF092}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bit" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,34 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
-  <si>
-    <t>Dor no peito</t>
-  </si>
-  <si>
-    <t>Boa circulação</t>
-  </si>
-  <si>
-    <t>Artéria bloqueada</t>
-  </si>
-  <si>
-    <t>Doença cardíaca</t>
-  </si>
-  <si>
-    <t>Não</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sim </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Não </t>
-  </si>
-  <si>
-    <t>Sim</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>H(p)</t>
   </si>
@@ -1349,24 +1321,24 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -1582,95 +1554,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>